<commit_message>
final testing - 2 success!!!
</commit_message>
<xml_diff>
--- a/output/extracted_data.xlsx
+++ b/output/extracted_data.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,647 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Invoice Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Invoice Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Supplier GST</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bill-To GST</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PO Number</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Address</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Seal &amp; Sign</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>No. of Items</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HSN/SAC</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Total Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IATIEN1819013538</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>15-02-2019</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>29AAHCS6672E1ZZ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>29AAFCA0924K1ZN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>WORKFELLA BUSINESS CENTRE, 1450/1, INFANTRY ROAD, OPP COMMISSIONER OFFICE, VASANTH NAGAR BENGALURU, 580001</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>FRONT WHEEL</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>70800</v>
+      </c>
+      <c r="N2" t="n">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>IATIEN1819013538</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15-02-2019</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>29AAHCS6672E1ZZ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>29AAFCA0924K1ZN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>WORKFELLA BUSINESS CENTRE, 1450/1, INFANTRY ROAD, OPP COMMISSIONER OFFICE, VASANTH NAGAR BENGALURU, 580001</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>ANO ADJUST</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>60000</v>
+      </c>
+      <c r="N3" t="n">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10-07-2014</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Client Address, City, State, Country ZIP CODE</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Item description goes here</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10-07-2014</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Client Address, City, State, Country ZIP CODE</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Item description goes here</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10-07-2014</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Client Address, City, State, Country ZIP CODE</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Item description goes hare</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10-07-2014</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Client Address, City, State, Country ZIP CODE</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Item description goes here</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2016-10014</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>09-11-2016</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>GB202208019</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>FR90103402210</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>581660</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>185 Portbello Rd, London WIE ILA, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Best of First Nibs 67 Cacao</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>7</v>
+      </c>
+      <c r="M8" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" t="n">
+        <v>69.65000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2016-10014</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>09-11-2016</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GB202208019</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FR90103402210</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>581660</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>185 Portbello Rd, London WIE ILA, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>O Pink sea sat 71 Cacao</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" t="n">
+        <v>20</v>
+      </c>
+      <c r="N9" t="n">
+        <v>23.85</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2016-10014</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>09-11-2016</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GB202208019</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FR90103402210</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>581660</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>185 Portbello Rd, London WIE ILA, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Maple and Nibs 75 Cacao</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>20</v>
+      </c>
+      <c r="N10" t="n">
+        <v>33.99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2016-10014</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>09-11-2016</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GB202208019</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>FR90103402210</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>581660</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>185 Portbello Rd, London WIE ILA, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>7 coconut Mink 60 Cacao</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>6</v>
+      </c>
+      <c r="M11" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" t="n">
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2016-10014</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09-11-2016</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GB202208019</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FR90103402210</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>581660</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>185 Portbello Rd, London WIE ILA, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>O Smoked Chat 66 Cacao</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
+        <v>4</v>
+      </c>
+      <c r="M12" t="n">
+        <v>20</v>
+      </c>
+      <c r="N12" t="n">
+        <v>31.8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>